<commit_message>
Modified label name add,edit monthly report
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample2test.xlsx
+++ b/public/assets/MonthlyReportSample2test.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Test Site</t>
   </si>
   <si>
-    <t xml:space="preserve">Site Type</t>
+    <t xml:space="preserve">Entry Point</t>
   </si>
   <si>
     <t xml:space="preserve">Facility</t>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Site Unique Id</t>
   </si>
   <si>
-    <t xml:space="preserve">Tester Name</t>
+    <t xml:space="preserve">Lab Manager Name</t>
   </si>
   <si>
     <t xml:space="preserve">Is FLC*</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Does site do Recency Tests?*</t>
   </si>
   <si>
-    <t xml:space="preserve">Tester Contact Number</t>
+    <t xml:space="preserve">Lab Manager Contact Number</t>
   </si>
   <si>
     <t xml:space="preserve">Algorithm Type </t>
@@ -335,11 +335,11 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z1" activeCellId="0" sqref="Z1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Check the duplicate entry in upload monthly report
</commit_message>
<xml_diff>
--- a/public/assets/MonthlyReportSample2test.xlsx
+++ b/public/assets/MonthlyReportSample2test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t xml:space="preserve">Test Site</t>
   </si>
@@ -139,19 +139,22 @@
     <t xml:space="preserve">16-6-2021</t>
   </si>
   <si>
+    <t xml:space="preserve">Jun-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test kit name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-6-2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test kit name2</t>
+  </si>
+  <si>
     <t xml:space="preserve">26-6-2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test kit name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26-6-2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test kit name2</t>
   </si>
 </sst>
 </file>
@@ -330,10 +333,10 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -505,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="AA2" s="7" t="n">
         <v>0</v>
@@ -529,7 +532,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>